<commit_message>
Assert for create share skill added, part of edit listing added.
</commit_message>
<xml_diff>
--- a/CompetitionMars/CompetitionMars/ExcelData/TestData.xlsx
+++ b/CompetitionMars/CompetitionMars/ExcelData/TestData.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\IC\Competition Mars\Project-Mars-Competition-task\CompetitionMars\CompetitionMars\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2DF8D60-072D-48EC-88B8-B76FDD872029}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B269E93D-393C-45FB-8B3C-EB96357CF8BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2064" yWindow="1512" windowWidth="19068" windowHeight="9456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SignIn" sheetId="1" r:id="rId1"/>
     <sheet name="SignUp" sheetId="2" r:id="rId2"/>
     <sheet name="CreateShareSkill" sheetId="3" r:id="rId3"/>
+    <sheet name="EditListing" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="45">
   <si>
     <t>FirstName</t>
   </si>
@@ -126,6 +127,42 @@
   </si>
   <si>
     <t>Active</t>
+  </si>
+  <si>
+    <t>Skill-Exchange</t>
+  </si>
+  <si>
+    <t>Testing exchange Tag</t>
+  </si>
+  <si>
+    <t>Hourly basis service</t>
+  </si>
+  <si>
+    <t>On-site</t>
+  </si>
+  <si>
+    <t>Skill-exchange</t>
+  </si>
+  <si>
+    <t>Hidden</t>
+  </si>
+  <si>
+    <t>Testing editing Title</t>
+  </si>
+  <si>
+    <t>Testing editing Description.</t>
+  </si>
+  <si>
+    <t>Testing editing Tag</t>
+  </si>
+  <si>
+    <t>Video &amp; Animation</t>
+  </si>
+  <si>
+    <t>Editing &amp; Post Production</t>
+  </si>
+  <si>
+    <t>Testing  editing exchange Tag</t>
   </si>
 </sst>
 </file>
@@ -574,10 +611,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF4A85CE-1B3B-4603-936F-1431CC5805B0}">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -595,10 +632,11 @@
     <col min="11" max="11" width="10.88671875" style="4" customWidth="1"/>
     <col min="12" max="12" width="11.44140625" style="4" customWidth="1"/>
     <col min="13" max="13" width="14.21875" style="4" customWidth="1"/>
-    <col min="14" max="16384" width="8.88671875" style="4"/>
+    <col min="14" max="14" width="19.44140625" style="4" customWidth="1"/>
+    <col min="15" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>10</v>
       </c>
@@ -639,10 +677,13 @@
         <v>30</v>
       </c>
       <c r="N1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="O1" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>21</v>
       </c>
@@ -682,12 +723,188 @@
       <c r="M2" s="4">
         <v>6</v>
       </c>
-      <c r="N2" s="6" t="s">
+      <c r="N2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="O2" s="6" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" s="8">
+        <v>45017</v>
+      </c>
+      <c r="I3" s="8">
+        <v>45118</v>
+      </c>
+      <c r="J3" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="K3" s="5">
+        <v>0.75</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="M3" s="4">
+        <v>6</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="O3" s="6" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07F231BA-E275-4E21-BA07-9D1241232B7A}">
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="22.5546875" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" customWidth="1"/>
+    <col min="3" max="3" width="17.21875" customWidth="1"/>
+    <col min="4" max="4" width="12.77734375" customWidth="1"/>
+    <col min="5" max="5" width="18.5546875" customWidth="1"/>
+    <col min="6" max="6" width="13.77734375" customWidth="1"/>
+    <col min="7" max="7" width="15.21875" customWidth="1"/>
+    <col min="8" max="8" width="19.21875" customWidth="1"/>
+    <col min="9" max="9" width="18" customWidth="1"/>
+    <col min="10" max="10" width="16.77734375" customWidth="1"/>
+    <col min="11" max="11" width="14.5546875" customWidth="1"/>
+    <col min="12" max="12" width="14.77734375" customWidth="1"/>
+    <col min="13" max="13" width="13.88671875" customWidth="1"/>
+    <col min="14" max="14" width="25.44140625" customWidth="1"/>
+    <col min="15" max="15" width="12.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" s="8">
+        <v>45414</v>
+      </c>
+      <c r="I2" s="8">
+        <v>45516</v>
+      </c>
+      <c r="J2" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="K2" s="5">
+        <v>0.75</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="M2" s="4">
+        <v>5</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
AutoIt added, Extent Report added.
</commit_message>
<xml_diff>
--- a/CompetitionMars/CompetitionMars/ExcelData/TestData.xlsx
+++ b/CompetitionMars/CompetitionMars/ExcelData/TestData.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\IC\Competition Mars\Project-Mars-Competition-task\CompetitionMars\CompetitionMars\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B269E93D-393C-45FB-8B3C-EB96357CF8BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC1C4397-A444-495D-82B1-C5EFCD9E9589}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2064" yWindow="1512" windowWidth="19068" windowHeight="9456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2172" yWindow="2520" windowWidth="19068" windowHeight="9456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SignIn" sheetId="1" r:id="rId1"/>
     <sheet name="SignUp" sheetId="2" r:id="rId2"/>
     <sheet name="CreateShareSkill" sheetId="3" r:id="rId3"/>
-    <sheet name="EditListing" sheetId="4" r:id="rId4"/>
+    <sheet name="EditListing" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="53">
   <si>
     <t>FirstName</t>
   </si>
@@ -147,15 +147,6 @@
     <t>Hidden</t>
   </si>
   <si>
-    <t>Testing editing Title</t>
-  </si>
-  <si>
-    <t>Testing editing Description.</t>
-  </si>
-  <si>
-    <t>Testing editing Tag</t>
-  </si>
-  <si>
     <t>Video &amp; Animation</t>
   </si>
   <si>
@@ -163,6 +154,39 @@
   </si>
   <si>
     <t>Testing  editing exchange Tag</t>
+  </si>
+  <si>
+    <t>Available Day</t>
+  </si>
+  <si>
+    <t>Tue</t>
+  </si>
+  <si>
+    <t>Wed</t>
+  </si>
+  <si>
+    <t>1200</t>
+  </si>
+  <si>
+    <t>1400</t>
+  </si>
+  <si>
+    <t>1800</t>
+  </si>
+  <si>
+    <t>1900</t>
+  </si>
+  <si>
+    <t>Fri</t>
+  </si>
+  <si>
+    <t>Testing Edit Title</t>
+  </si>
+  <si>
+    <t>Testing Editing Description.</t>
+  </si>
+  <si>
+    <t>Testing editing tag</t>
   </si>
 </sst>
 </file>
@@ -220,7 +244,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -228,12 +252,16 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -611,10 +639,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF4A85CE-1B3B-4603-936F-1431CC5805B0}">
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:P3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection sqref="A1:P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -627,16 +655,16 @@
     <col min="6" max="6" width="15.5546875" style="4" customWidth="1"/>
     <col min="7" max="7" width="14.33203125" style="4" customWidth="1"/>
     <col min="8" max="8" width="18.21875" style="4" customWidth="1"/>
-    <col min="9" max="9" width="13.77734375" style="4" customWidth="1"/>
-    <col min="10" max="10" width="11.109375" style="4" customWidth="1"/>
-    <col min="11" max="11" width="10.88671875" style="4" customWidth="1"/>
-    <col min="12" max="12" width="11.44140625" style="4" customWidth="1"/>
-    <col min="13" max="13" width="14.21875" style="4" customWidth="1"/>
-    <col min="14" max="14" width="19.44140625" style="4" customWidth="1"/>
-    <col min="15" max="16384" width="8.88671875" style="4"/>
+    <col min="9" max="10" width="13.77734375" style="4" customWidth="1"/>
+    <col min="11" max="11" width="11.109375" style="9" customWidth="1"/>
+    <col min="12" max="12" width="10.88671875" style="9" customWidth="1"/>
+    <col min="13" max="13" width="11.44140625" style="4" customWidth="1"/>
+    <col min="14" max="14" width="14.21875" style="4" customWidth="1"/>
+    <col min="15" max="15" width="19.44140625" style="4" customWidth="1"/>
+    <col min="16" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>10</v>
       </c>
@@ -665,35 +693,38 @@
         <v>20</v>
       </c>
       <c r="J1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="K1" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>23</v>
       </c>
       <c r="E2" s="4" t="s">
@@ -705,42 +736,45 @@
       <c r="G2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="8">
+      <c r="H2" s="7">
         <v>45017</v>
       </c>
-      <c r="I2" s="8">
+      <c r="I2" s="7">
         <v>45118</v>
       </c>
-      <c r="J2" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="K2" s="5">
-        <v>0.75</v>
-      </c>
-      <c r="L2" s="4" t="s">
+      <c r="J2" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="M2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="M2" s="4">
+      <c r="N2" s="4">
         <v>6</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="O2" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="O2" s="6" t="s">
+      <c r="P2" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="6" t="s">
         <v>23</v>
       </c>
       <c r="E3" s="4" t="s">
@@ -752,28 +786,31 @@
       <c r="G3" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="H3" s="8">
+      <c r="H3" s="7">
         <v>45017</v>
       </c>
-      <c r="I3" s="8">
+      <c r="I3" s="7">
         <v>45118</v>
       </c>
-      <c r="J3" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="K3" s="5">
-        <v>0.75</v>
-      </c>
-      <c r="L3" s="4" t="s">
+      <c r="J3" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="K3" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="L3" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="M3" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="M3" s="4">
+      <c r="N3" s="4">
         <v>6</v>
       </c>
-      <c r="N3" s="4" t="s">
+      <c r="O3" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="O3" s="6" t="s">
+      <c r="P3" s="5" t="s">
         <v>38</v>
       </c>
     </row>
@@ -784,33 +821,34 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07F231BA-E275-4E21-BA07-9D1241232B7A}">
-  <dimension ref="A1:O2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5A2DA08-D9AF-47D5-AEBE-1EFAA4F0A99C}">
+  <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.5546875" customWidth="1"/>
-    <col min="2" max="2" width="23.33203125" customWidth="1"/>
-    <col min="3" max="3" width="17.21875" customWidth="1"/>
-    <col min="4" max="4" width="12.77734375" customWidth="1"/>
-    <col min="5" max="5" width="18.5546875" customWidth="1"/>
-    <col min="6" max="6" width="13.77734375" customWidth="1"/>
-    <col min="7" max="7" width="15.21875" customWidth="1"/>
-    <col min="8" max="8" width="19.21875" customWidth="1"/>
-    <col min="9" max="9" width="18" customWidth="1"/>
-    <col min="10" max="10" width="16.77734375" customWidth="1"/>
-    <col min="11" max="11" width="14.5546875" customWidth="1"/>
-    <col min="12" max="12" width="14.77734375" customWidth="1"/>
-    <col min="13" max="13" width="13.88671875" customWidth="1"/>
-    <col min="14" max="14" width="25.44140625" customWidth="1"/>
-    <col min="15" max="15" width="12.88671875" customWidth="1"/>
+    <col min="1" max="1" width="15.21875" customWidth="1"/>
+    <col min="2" max="2" width="25.44140625" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" customWidth="1"/>
+    <col min="4" max="4" width="21.6640625" customWidth="1"/>
+    <col min="5" max="5" width="16.44140625" customWidth="1"/>
+    <col min="6" max="6" width="17.109375" customWidth="1"/>
+    <col min="7" max="7" width="13.88671875" customWidth="1"/>
+    <col min="8" max="8" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" customWidth="1"/>
+    <col min="10" max="10" width="11.5546875" customWidth="1"/>
+    <col min="11" max="11" width="13.33203125" customWidth="1"/>
+    <col min="12" max="12" width="14.88671875" customWidth="1"/>
+    <col min="13" max="13" width="12.5546875" customWidth="1"/>
+    <col min="14" max="14" width="15.33203125" customWidth="1"/>
+    <col min="15" max="15" width="25.6640625" customWidth="1"/>
+    <col min="16" max="16" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>10</v>
       </c>
@@ -839,68 +877,74 @@
         <v>20</v>
       </c>
       <c r="J1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="K1" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="D2" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" s="10">
+        <v>45414</v>
+      </c>
+      <c r="I2" s="10">
+        <v>45516</v>
+      </c>
+      <c r="J2" t="s">
+        <v>49</v>
+      </c>
+      <c r="K2">
+        <v>1300</v>
+      </c>
+      <c r="L2">
+        <v>1500</v>
+      </c>
+      <c r="M2" t="s">
+        <v>37</v>
+      </c>
+      <c r="N2">
+        <v>5</v>
+      </c>
+      <c r="O2" t="s">
         <v>41</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H2" s="8">
-        <v>45414</v>
-      </c>
-      <c r="I2" s="8">
-        <v>45516</v>
-      </c>
-      <c r="J2" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="K2" s="5">
-        <v>0.75</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="M2" s="4">
-        <v>5</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="O2" s="6" t="s">
+      <c r="P2" t="s">
         <v>38</v>
       </c>
     </row>

</xml_diff>